<commit_message>
add responses to excel, only unique ones
</commit_message>
<xml_diff>
--- a/db/forms-data.xlsx
+++ b/db/forms-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u130035\Desktop\pc-status-website\pc-status-website\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386905DA-B8A6-4AF7-80AF-8F1FC19B053E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CB6FD0-ABC7-4D73-927A-0FCE799584ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>שם מלא</t>
   </si>
@@ -51,26 +51,34 @@
     <t>מייל אזרחי</t>
   </si>
   <si>
-    <t>מס' טלפון</t>
-  </si>
-  <si>
     <t>הערות</t>
   </si>
   <si>
     <t>תאריך כניסת מחשב</t>
+  </si>
+  <si>
+    <t>טלפון אזרחי</t>
+  </si>
+  <si>
+    <t>סטטוס</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,7 +89,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -89,17 +97,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -113,9 +191,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{85F57428-87F0-431A-B472-1D3B38247708}" name="טבלה1" displayName="טבלה1" ref="A1:K2" totalsRowShown="0">
-  <autoFilter ref="A1:K2" xr:uid="{2F0398F1-3CF9-4C2B-8B79-4A4840CD065C}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{85F57428-87F0-431A-B472-1D3B38247708}" name="טבלה1" displayName="טבלה1" ref="A1:L2" insertRow="1" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1">
+  <autoFilter ref="A1:L2" xr:uid="{2F0398F1-3CF9-4C2B-8B79-4A4840CD065C}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{090ACBF1-143E-4BA1-9FED-7ED049DE281E}" name="שם מלא"/>
     <tableColumn id="2" xr3:uid="{BB8B126B-95C8-4478-B4F7-EFE26F348188}" name="תאריך כניסת מחשב"/>
     <tableColumn id="3" xr3:uid="{5CBCC541-2E96-4134-B094-E3C46FFE2E83}" name="הפעולה הנדרשת"/>
@@ -125,8 +203,9 @@
     <tableColumn id="7" xr3:uid="{86C41F43-91D1-4BA2-8003-A9BBA61F515E}" name="יחידה"/>
     <tableColumn id="8" xr3:uid="{72ABF582-6CF4-4126-B04A-243CFE7F846F}" name="מספר אישי/ת.ז"/>
     <tableColumn id="9" xr3:uid="{481D0390-E6F3-43BC-AF5F-7C480109406D}" name="מייל אזרחי"/>
-    <tableColumn id="10" xr3:uid="{F00463F2-9701-4369-83E5-56DA09B583C8}" name="מס' טלפון"/>
+    <tableColumn id="10" xr3:uid="{F00463F2-9701-4369-83E5-56DA09B583C8}" name="טלפון אזרחי"/>
     <tableColumn id="11" xr3:uid="{29889D2D-81B6-4633-9C65-4E66A3A69603}" name="הערות"/>
+    <tableColumn id="12" xr3:uid="{FE80E4D6-E873-4166-835D-B9975EDD35FC}" name="סטטוס"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -395,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,39 +495,42 @@
     <col min="11" max="11" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>